<commit_message>
new programs added MIT and PY4E
</commit_message>
<xml_diff>
--- a/ComputerScience/CS Timeline Estimate degree.xlsx
+++ b/ComputerScience/CS Timeline Estimate degree.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\OSSU\ComputerScience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\OSSU\ComputerScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF2FF17-1955-4FFD-A348-174001286C0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A92118E4-A861-412D-A62A-F494336A9751}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,10 +578,10 @@
     <t>Advanced Applications 8</t>
   </si>
   <si>
-    <t>Lesson 3 Vid 2</t>
-  </si>
-  <si>
-    <t>Download Py</t>
+    <t>Lecture 2 Vid 3</t>
+  </si>
+  <si>
+    <t>Lesson 4</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
     <numFmt numFmtId="165" formatCode="yyyy&quot; &quot;mmm&quot; &quot;dd"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -747,6 +747,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -793,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -919,6 +925,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2446,10 +2453,10 @@
   <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2545,8 +2552,8 @@
         <v>44291</v>
       </c>
       <c r="K2" s="18"/>
-      <c r="L2" s="24" t="s">
-        <v>185</v>
+      <c r="L2" s="49" t="s">
+        <v>186</v>
       </c>
       <c r="M2" s="45"/>
     </row>
@@ -2587,7 +2594,7 @@
       </c>
       <c r="K3" s="18"/>
       <c r="L3" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M3" s="46" t="s">
         <v>21</v>

</xml_diff>